<commit_message>
create login with sqlite
</commit_message>
<xml_diff>
--- a/sales_data.xlsx
+++ b/sales_data.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>leo</t>
+  </si>
+  <si>
+    <t>teste</t>
   </si>
   <si>
     <t>Sales</t>
@@ -371,15 +374,15 @@
         <v>1000</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>500</v>
@@ -387,7 +390,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>500</v>

</xml_diff>